<commit_message>
Leads Module added in Master file.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BCB8D36F-EEF3-4AE5-9551-FEDCDA8CC16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AFF18B87-0E59-418D-AB35-7CD72FD4546D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="1" r:id="rId1"/>
     <sheet name="Contact" sheetId="2" r:id="rId2"/>
-    <sheet name="Product" sheetId="3" r:id="rId3"/>
-    <sheet name="DataProviderOrg" sheetId="4" r:id="rId4"/>
+    <sheet name="Leads" sheetId="5" r:id="rId3"/>
+    <sheet name="Product" sheetId="3" r:id="rId4"/>
+    <sheet name="DataProviderOrg" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I10"/>
+  <oleSize ref="A1:J11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>TC_ID</t>
   </si>
@@ -126,6 +127,27 @@
   </si>
   <si>
     <t>RealMe</t>
+  </si>
+  <si>
+    <t>CreateLeads</t>
+  </si>
+  <si>
+    <t>CreateLeadsWithLeadSource</t>
+  </si>
+  <si>
+    <t>Kat</t>
+  </si>
+  <si>
+    <t>Lead Source</t>
+  </si>
+  <si>
+    <t>Cold Call</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Kay Beauty</t>
   </si>
 </sst>
 </file>
@@ -167,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -190,15 +212,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590B7557-1150-4C90-BF4A-2C91F83F8663}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="122" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,6 +670,88 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB308AAF-152C-4E95-9FBE-4FA304ABAD52}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -713,7 +829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAEFBF-0003-4C1C-934E-6C3A3B4F37D9}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>